<commit_message>
data set is updated
</commit_message>
<xml_diff>
--- a/final_data1.xlsx
+++ b/final_data1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wayamba University\Level_4 Sem_1\CMIS 4†26 - Project\Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Drive\CMIS 4†26 - Project\Data Set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969046BA-7901-48A0-ACAC-85DEFDD62514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71BD021-A8A1-45A0-B9AC-88DCC34AFF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1909,13 +1909,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="G147" sqref="G147"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.33203125" customWidth="1"/>
     <col min="5" max="5" width="16.88671875" customWidth="1"/>
     <col min="6" max="6" width="16.5546875" customWidth="1"/>

</xml_diff>